<commit_message>
top 10 search res
</commit_message>
<xml_diff>
--- a/zara_search_results.xlsx
+++ b/zara_search_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>WebIndustria de Diseño Textil, S.A. (INDITEX, S.A.) Avenida de la Diputación, Edificio Inditex, 15143, Arteixo (A Coruña), Spain. Latest trends in clothing for women, men &amp; kids at …</t>
+          <t>WebWe are present in over 156 stores, please select yours. here. Latest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; …</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>WebZARA is a global fashion brand that offers clothing, shoes and accessories for men, women and kids. Choose your country and language to browse the latest collections and shop …</t>
+          <t>WebZARA Official Website. Presione enter para accesibilidad para personas ciegas. Presione enter para navegar por el teclado. Presione enter para acceder al menú de accesibilidad. …</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,17 +502,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Women's Special Prices | Explore our New Arrivals | ZARA India</t>
+          <t>Women's New In Clothes | Explore our New Arrivals | ZARA India</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/woman-special-prices-l1314.html</t>
+          <t>https://www.zara.com/in/en/woman-new-in-l1180.html</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>WebThe Zara special prices edit is perfect for finding that one thing your wardrobe is missing, whether it be a little black dress, blazer, a pair of jeans, or staples like vests, T-shirts and …</t>
+          <t>Webzara origins NEW; edition NEW; #selectedby NEW /// new; jackets; puffers; trousers; jeans; sweaters | cardigans; hoodies | sweatshirts; t-shirts; overshirts; shirts; polo shirts; linen; …</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -524,17 +524,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ZARA International | New Collection Online</t>
+          <t>Women's Jackets | ZARA India</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.zara.com/ww/</t>
+          <t>https://www.zara.com/in/en/woman-jackets-l1114.html</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>WebLatest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
+          <t>WebZARA's women's jackets and waistcoats are easy to wear and complement any look. Our women's corduroy jackets will keep the cold at bay and add instant edge to any outfit, …</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,17 +546,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ZW COLLECTION MANTECO WOOL BLEND COAT WITH …</t>
+          <t>LEATHER JACKET - Dark brown | ZARA India</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/zw-collection-manteco-wool-blend-coat-with-toggles-p02111741.html</t>
+          <t>https://www.zara.com/in/en/leather-jacket-p02521105.html</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>WebSUMMERY GARMENTS. ZARA ATHLETICZ. ZARA ORIGINS. SPECIAL EDITION. + Info. ZARA WOMAN COLLECTION Oversize coat made of a spun Manteco wool blend. …</t>
+          <t>WebCropped fit jacket made of leather treated with a process that gives it a creased appearance. Lapel collar and long sleeves. Hip welt pockets and interior pocket detail. Front zip …</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,17 +568,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>STRETCH ANKLE BOOTS - Black | ZARA India</t>
+          <t>Women's Handbags | Explore our New Arrivals | ZARA India</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/stretch-ankle-boots-p12103330.html</t>
+          <t>https://www.zara.com/in/en/woman-bags-handbags-l1037.html</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>WebStretch ankle boots with knit detail on the leg. Zip closure. Front and back pull tab for slipping on with ease. Flexible insole. Chunky rubber track sole. SIZE 40: shoes …</t>
+          <t>WebWomen’s handbags come in all shapes for this season, from the traditional to the unexpected. Vintage silhouettes such as Nineties shoulder bags and Fifties top handle …</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -590,17 +590,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Women's Clothes | ZARA United States</t>
+          <t>Dresses for Women | ZARA India</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.zara.com/us/en/woman-mkt1000.html</t>
+          <t>https://www.zara.com/in/en/woman-dresses-l1066.html</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>WebShop online for the latest trends in women's fashion at ZARA. Enjoy free shipping and try on at your leisure with no minimum purchase.</t>
+          <t>WebZARA's short dresses include both classic and on-trend styles. The short black dress, also known as little black dress, is an emblematic garment basic for any woman's wardrobe. One of its many qualities is not only the great potential in terms of versatility; it is a piece that exudes unpretentious elegance wherever it goes.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,17 +612,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Men´s Clothes | ZARA India</t>
+          <t>Women's Clothes | ZARA United Kingdom</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/man-mkt534.html</t>
+          <t>https://www.zara.com/uk/en/woman-mkt1000.html</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>WebThe latest clothes, shoes and accessories for men every week at ZARA online. Enter now and discover all the shirts of the new collection</t>
+          <t>WebWeekly new trends in clothes, shoes &amp; accessories at ZARA online. FREE SHIPPING* for you to try on at your leisure.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,17 +634,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ZARA Canada | New Collection Online</t>
+          <t>Men´s Clothes | ZARA India</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.zara.com/ca/</t>
+          <t>https://www.zara.com/in/en/man-mkt534.html</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>WebDiscover the new ZARA collection online. The latest trends for Woman, Man, Kids and next season’s ad campaigns.</t>
+          <t>WebThe latest clothes, shoes and accessories for men every week at ZARA online. Enter now and discover all the shirts of the new collection</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -656,17 +656,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ZARA Australia | New Collection Online</t>
+          <t>Women's Just In Clothes | Explore our New Arrivals - ZARA</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.zara.com/au/</t>
+          <t>https://www.zara.com/us/en/woman-new-in-l1180.html</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>WebLatest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
+          <t>WebFREE SHIPPING. New clothes and accessories updated weekly at ZARA online. Stay in style with seasonal trends.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -678,17 +678,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Dresses for Women | Explore our New Arrivals | ZARA United …</t>
+          <t>ZARA Canada | New Collection Online</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.zara.com/us/en/woman-dresses-l1066.html</t>
+          <t>https://www.zara.com/ca/</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>WebZara's women's dresses collection comprises a wide variety of styles. From the latest arrivals to pieces for a basic wardrobe, both on-trend and timeless designs are featured in the collection. A black dress represents the highest level of elegance. Zara's selection includes different alternatives to the iconic little black dress, a key piece ...</t>
+          <t>WebDiscover the new ZARA collection online. The latest trends for Woman, Man, Kids and next season’s ad campaigns.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -700,17 +700,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Women's Special Prices | Explore our New Arrivals | ZARA India</t>
+          <t>ZARA Philippines | New Collection Online</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/woman-special-prices-l1314.html</t>
+          <t>https://www.zara.com/ph/</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>WebThe Zara special prices edit is perfect for finding that one thing your wardrobe is missing, whether it be a little black dress, blazer, a pair of jeans, or staples like vests, T-shirts and lingerie. Available in store and online, shop clothes, accessories and footwear on sale. ZW COLLECTION SHORT WOOL BLEND COAT ₹ 13,990.00-42 % ₹ 7,990.00. WOOL AND …</t>
+          <t>WebLatest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -722,17 +722,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ZARA Philippines | New Collection Online</t>
+          <t>Dresses for Women | ZARA United States</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.zara.com/ph/</t>
+          <t>https://www.zara.com/us/en/woman-dresses-l1066.html</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>WebHello, Yes, continue on Philippines. Yes, continue on Philippines. No, go to the website for United States. We are present in over 156 stores, please select yours. Latest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
+          <t>WebZara's women's dresses collection comprises a wide variety of styles. From the latest arrivals to pieces for a basic wardrobe, both on-trend and timeless designs are featured in the collection. A black dress represents the highest level of elegance. Zara's selection includes different alternatives to the iconic little black dress, a key piece ...</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -744,17 +744,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ZARA Official Website</t>
+          <t>Men´s New In Clothes | Explore our New Arrivals | ZARA India</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.zara.com/</t>
+          <t>https://www.zara.com/in/en/man-new-in-l711.html</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>WebZARA Official Website. Presione enter para accesibilidad para personas ciegas. Presione enter para navegar por el teclado. Presione enter para acceder al menú de accesibilidad. United States. English. Go. Albania Algérie Andorra Angola Armenia Argentina Aruba Australia Azerbaijan Bahrain Belgium Беларусь/Belarus Bosnia And Herzegovina ...</t>
+          <t>WebOur edit of new men's clothes takes in timeless wardrobe heroes and new trends in fashion. From staples - including T-shirts, vests, knitwear, sleepwear and underwear - to smart occasionwear, such as shirts, blazers and co-ord suits, the complete closet has been considered and is waiting to shop online.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -766,17 +766,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Kid´s Clothes | ZARA India</t>
+          <t>Women's Special Prices | Explore our New Arrivals | ZARA India</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/kids-mkt1.html</t>
+          <t>https://www.zara.com/in/en/woman-special-prices-l1314.html</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>WebDiscover the latest kids' clothes, shoes and accessories updated every week at ZARA online.</t>
+          <t>WebThe Zara special prices edit is perfect for finding that one thing your wardrobe is missing, whether it be a little black dress, blazer, a pair of jeans, or staples like vests, T-shirts and lingerie. Available in store and online, shop clothes, accessories and footwear on sale. TURTLENECK SWEATER +3 ₹ 2,290.00-30 % ₹ 1,590.00. TURTLENECK SWEATER …</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -788,12 +788,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ZARA United Kingdom | New Collection Online</t>
+          <t>ZARA UAE - Dubai/Sharjah/Ajman/UAQ/Fujairah | New …</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://www.zara.com/uk/</t>
+          <t>https://www.zara.com/ae/</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -810,17 +810,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ZARA Saudi Arabia | New Collection Online</t>
+          <t>Women's Trousers | ZARA India</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.zara.com/sa/en/</t>
+          <t>https://www.zara.com/in/en/woman-trousers-l1335.html</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>WebYes, continue on Saudi Arabia. No, go to the website for United States. We are present in over 156 stores, please select yours. here. Latest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
+          <t>WebZARA's collection of women's trousers connects every woman to her ideal fit. The wide variety of cuts and styles allows you to create a versatile wardrobe with trousers for every occasion. Women's dress trousers are one of the most flattering garments: they are slimming and offer the possibility to select the right fit for each body type.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -832,17 +832,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Women's Jackets | Explore our New Arrivals | ZARA India</t>
+          <t>ZARA Ireland | New Collection Online</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/woman-jackets-l1114.html</t>
+          <t>https://www.zara.com/ie/</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>WebFrom practical women's denim jackets and military jackets to delicate options with special textures such as women's openwork jackets, party jackets or kimono style jackets. ZARA's women's jackets and waistcoats are easy to wear and complement any look. Our women's corduroy jackets will keep the cold at bay and add instant edge to any outfit ...</t>
+          <t>WebLatest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -854,12 +854,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ZARA UAE - Dubai/Sharjah/Ajman/UAQ/Fujairah | New …</t>
+          <t>ZARA Hungary / Hungary | New Collection Online</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.zara.com/ae/</t>
+          <t>https://www.zara.com/hu/</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -876,17 +876,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ZARA Germany | New Collection Online</t>
+          <t>Women's Jackets | ZARA India</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.zara.com/de/en/</t>
+          <t>https://www.zara.com/in/en/woman-jackets-l1114.html</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>WebLatest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
+          <t>WebZARA's women's jackets and waistcoats are easy to wear and complement any look. Our women's corduroy jackets will keep the cold at bay and add instant edge to any outfit, thanks to their soft ribbed fabric which lasts in every wardrobe through the seasons. Meanwhile, our iconic women's leather jackets, regardless of their fit, are timeless ...</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -898,17 +898,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ZARA Hrvatska / Croatia | Nova kolekcija online</t>
+          <t>ZARA Saudi Arabia | New Collection Online</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.zara.com/hr/</t>
+          <t>https://www.zara.com/sa/en/</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>WebOtkrijte novu kolekciju trgovine ZARA online. Posljednji trendovi za žene, muškarce i djecu te modni editorijali za nadolazeću sezonu.</t>
+          <t>WebYes, continue on Saudi Arabia. No, go to the website for United States. We are present in over 156 stores, please select yours. here. Latest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -920,17 +920,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Men´s Clothing | ZARA United States</t>
+          <t>Women's New In Clothes | Explore our New Arrivals - ZARA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.zara.com/us/en/man-mkt534.html</t>
+          <t>https://www.zara.com/uk/en/woman-new-in-l1180.html</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>WebThe latest clothes, shoes and accessories for men every week at ZARA . Discover men's clothing collection, from basics to trendy styles, find the perfect item for any occasion. Please note: This website includes an accessibility system. Press Control-F11 to adjust the website to the visually impaired who are using a screen reader; Press Control-F10 to …</t>
+          <t>WebNew clothes and accessories updated weekly at ZARA online. Stay in style with seasonal trends.</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -942,17 +942,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Men's Faux Leather Jackets | Explore our New Arrivals - ZARA</t>
+          <t>Women's Blazers | ZARA India</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/man-jackets-faux-leather-l650.html</t>
+          <t>https://www.zara.com/in/en/woman-blazers-l1055.html</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>WebFaux-Leather Jackets For Men. Articulated design and textile technology give our collection of comfortable faux-leather jackets an edge. From pared-back and relaxed designs to more experimental pieces, a faux-leather jacket has fuss-free appeal. Biker, tailored and bomber silhouettes are complemented by black, cream, brown and multicoloured ...</t>
+          <t>WebZara offers a collection of women's blazers that focuses on the original silhouette of this jacket, including updated proposals as well as classic designs that never go out of fashion. For a sophisticated, seamless look, the black blazer and the white blazer have a special place. As contemporary alternatives, the cropped and oversize blazer carry the …</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -964,17 +964,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Women's Crop Tops | Explore our New Arrivals | ZARA India</t>
+          <t>Women's T-shirts | ZARA India</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/woman-tops-crop-l1584.html</t>
+          <t>https://www.zara.com/in/en/woman-tshirts-l1362.html</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>WebName and address of the manufacturer: Industria de Diseño Textil, S.A. (INDITEX, S.A.) Avenida de la Diputación, Edificio Inditex, 15143, Arteixo (A Coruña), Spain</t>
+          <t>WebThis collection of women's T-shirts from Zara pays tribute to an everyday garment that holds a special place in women's wardrobes. Black and white T-shirts are neutral and adaptable, which makes them suitable for a wide range of styles, while oversized and cropped T-shirts add an urban touch to casual looks. In addition, this garment is also suitable for delicate …</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -986,17 +986,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ZARA Malaysia | New Collection Online</t>
+          <t>ZARA North Macedonia | New Collection Online</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.zara.com/my/</t>
+          <t>https://www.zara.com/mk/en/</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>WebLatest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
+          <t>WebHello, Yes, continue on North Macedonia. Yes, continue on North Macedonia. No, go to the website for United States. We are present in over 156 stores, please select yours. here. Latest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1008,262 +1008,20 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>| Explore our New Arrivals | ZARA India</t>
+          <t>Women's Tops | ZARA India</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.zara.com/in/en/woman-basics-l1050.html</t>
+          <t>https://www.zara.com/in/en/woman-tops-l1322.html</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>WebZARA WOMAN COLLECTION ₹ 8,590.00-53 % ₹ 3,990.00. ZW COLLECTION STRAIGHT LEG MID-RISE CROPPED JEANS. Slim Fit - Straight Leg - Mid Rise ₹ 3,290.00. WIDE-LEG PLUSH TROUSERS. High-waist trousers made of a cotton blend. Adjustable elasticated waistband with drawstrings. Pronounced seams. ₹ 2,290.00. COTTON AND MODAL …</t>
+          <t>WebTops For Women. Our collection of women’s tops has something to balance with every outfit, whether you prefer off-the-shoulder styles, halternecks, camisoles or knitted jersey t-shirts. Classic black, white, pink and navy block colours sit alongside everything from sequin tops to statement animal prints, to original slogan T-shirts this season.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>ZARA Netherlands | New Collection Online</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/nl/</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>WebZARA Nederland / Netherlands | Nieuwe Collectie Online. Kleding voor dames, heren, meisjes, jongens en baby´s in de ZARA online shop. Trends, catalogus, collectie en lookbooks elke week online bij ZARA.</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Women's Blazers | Explore our New Arrivals | ZARA India</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/in/en/woman-blazers-l1055.html</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>WebZara offers a collection of women's blazers that focuses on the original silhouette of this jacket, including updated proposals as well as classic designs that never go out of fashion. For a sophisticated, seamless look, the black blazer and the white blazer have a special place. As contemporary alternatives, the cropped and oversize blazer carry the …</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>ZARA South Africa | New Collection Online</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/za/</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>WebYes, continue on South Africa. Yes, continue on South Africa. No, go to the website for United States. We are present in over 156 stores, please select yours. Latest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Zara (retailer) - Wikipedia</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Zara_(retailer)</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>WebZARA (Spanish:) is a Spanish multinational retail clothing chain. It specializes in fast fashion and sells clothing, accessories, shoes, beauty products and perfumes. The head office is located at Arteixo in the province of A Coruña, Galicia. It is the largest constituent company of the Inditex group. In 2020, it was launching over twenty new product lines per year. …</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Women's Tops | ZARA India</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/in/en/woman-tops-l1322.html</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>WebWoman Tops. Our women’s tops cater to all occasions, tastes, styles and silhouettes to ensure there is something for every wardrobe.T-shirts come in long-sleeved, short-sleeved and cropped options, while vests and camisoles have been designed with both skinny straps and thick straps to offer variety. Blouses come in many different designs ...</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Women's Accessories | ZARA India</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/in/en/woman-accessories-l1003.html</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>WebName and address of the manufacturer: Industria de Diseño Textil, S.A. (INDITEX, S.A.) Avenida de la Diputación, Edificio Inditex, 15143, Arteixo (A Coruña), Spain</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>ZARA Ireland | New Collection Online</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/ie/</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>WebLatest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Special Prices Man | ZARA India</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/in/en/man-special-prices-l806.html</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>WebName and address of the manufacturer: Industria de Diseño Textil, S.A. (INDITEX, S.A.) Avenida de la Diputación, Edificio Inditex, 15143, Arteixo (A Coruña), Spain</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Women's Shoes | ZARA India</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/in/en/woman-shoes-l1251.html</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>WebZARA's proposal of sneakers for women manages to give a touch of modernity to the most formal garments and adds a touch of style to any look. ZARA's designs of women's sneakers are also ideal for combining with office clothing, as they are available in elegant styles and neutral colors. High-heeled shoes are a basic that withstands the passage ...</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Women's Outerwear | ZARA India</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/in/en/woman-outerwear-l1184.html</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>WebZARA presents its fashionable coat edit, based on variety. This edit includes cold and rainy weather essentials such as anoraks, quilted gilets and of course, waterproof coats with hoods.There are also cloth coats which add a touch of finesse and warmth, and women's jackets with an adaptable, versatile design that are a must-have in every wardrobe.</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>ZARA Hungary / Hungary | New Collection Online</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>https://www.zara.com/hu/</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>WebLatest trends in clothing for women, men &amp; kids at ZARA online. Find new arrivals, fashion catalogs, collections &amp; lookbooks every week.</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>